<commit_message>
Updates to calibrate buildings and transportation sector (pulled data from prior Hong Kong model and added in data for motorbikes, freight). Removed an extra file.
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Desktop\eps-1.4.3-hong-kong-wipB\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Pre-Calibration Calculated Vals" sheetId="7" r:id="rId6"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="381">
   <si>
     <t>SoCEUtiNTY Share of Components Energy Use that is New This Year</t>
   </si>
@@ -1168,9 +1168,6 @@
   </si>
   <si>
     <t>This variable may need to be recalibrated when adapting the model</t>
-  </si>
-  <si>
-    <t>Share of New Components Energy Use (dimensionless)</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1340,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1412,9 +1409,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1731,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1743,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1756,92 +1750,92 @@
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B5" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B10" s="30" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="30" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="30" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B25" s="33" t="s">
         <v>372</v>
       </c>
@@ -1886,32 +1880,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>379</v>
       </c>
@@ -26347,7 +26341,9 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26357,10 +26353,7 @@
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>381</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="27" t="s">
         <v>353</v>
       </c>
@@ -26376,14 +26369,14 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>4.5699999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C2" s="4">
         <f>B2</f>
-        <v>4.5699999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>4.7800000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26391,14 +26384,14 @@
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>5.7000000000000002E-2</v>
+        <v>6.1199999999999997E-2</v>
       </c>
       <c r="C3" s="4">
         <f>B3</f>
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="D3" s="34">
         <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="D3" s="34">
-        <v>6.2E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26420,14 +26413,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="34">
-        <v>0.114</v>
+        <v>0.111</v>
       </c>
       <c r="C5" s="4">
         <f>B5</f>
-        <v>0.114</v>
+        <v>0.111</v>
       </c>
       <c r="D5" s="34">
-        <v>0.112</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26435,14 +26428,14 @@
         <v>7</v>
       </c>
       <c r="B6" s="34">
-        <v>7.1499999999999994E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="C6" s="4">
         <f>B6</f>
-        <v>7.1499999999999994E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D6" s="34">
-        <v>7.1199999999999999E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26450,14 +26443,14 @@
         <v>8</v>
       </c>
       <c r="B7" s="34">
-        <v>6.7500000000000004E-2</v>
+        <v>6.6400000000000001E-2</v>
       </c>
       <c r="C7" s="4">
         <f>B7</f>
-        <v>6.7500000000000004E-2</v>
+        <v>6.6400000000000001E-2</v>
       </c>
       <c r="D7" s="34">
-        <v>6.9500000000000006E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -26703,6 +26696,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -26711,23 +26713,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4FF5AC-9675-44D2-942C-C25B007B773B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04533B93-14EF-4EC4-AADF-C1C2F3C700CC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A758CE-E65C-4D47-9536-08378DBB5615}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{168006FD-5661-4E7D-9F50-743F4C0D0570}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFBF401-06C6-407D-B830-EB8100B5526F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C7C53D5-F759-46CC-8857-FF43092E2A2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>